<commit_message>
geneva position conversion added
</commit_message>
<xml_diff>
--- a/samples/Repo Exposure Trades and Collateral Position.xlsx
+++ b/samples/Repo Exposure Trades and Collateral Position.xlsx
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\hsbc_repo\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC94715-C5FB-4692-ACB0-28562B41C4AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CC7C8A-F93A-4E89-8FCB-BB7D48A2E5C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pNonCSV_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -280,9 +288,6 @@
     <t>ORIEAS 0 12/21/20</t>
   </si>
   <si>
-    <t>XS1692178665</t>
-  </si>
-  <si>
     <t>AQ4029965</t>
   </si>
   <si>
@@ -313,6 +318,9 @@
   </si>
   <si>
     <t>RESTRICTED</t>
+  </si>
+  <si>
+    <t>XS9999998888</t>
   </si>
 </sst>
 </file>
@@ -499,29 +507,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -889,7 +897,7 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:R25"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -902,10 +910,10 @@
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="12.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -916,65 +924,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29.25" customHeight="1">
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:20">
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
@@ -993,80 +1001,80 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="19" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="16"/>
+      <c r="I9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="19" t="s">
+      <c r="J9" s="16"/>
+      <c r="K9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="19" t="s">
+      <c r="L9" s="16"/>
+      <c r="M9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="12"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1084,52 +1092,52 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="12"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="16"/>
       <c r="S10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="3" t="s">
@@ -1224,7 +1232,7 @@
       <c r="J13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="9" t="s">
         <v>46</v>
       </c>
       <c r="L13" s="5" t="s">
@@ -1286,7 +1294,7 @@
       <c r="J14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="9" t="s">
         <v>50</v>
       </c>
       <c r="L14" s="5" t="s">
@@ -1782,7 +1790,7 @@
       <c r="J22" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="9" t="s">
         <v>82</v>
       </c>
       <c r="L22" s="5" t="s">
@@ -1841,14 +1849,14 @@
       <c r="I23" s="8">
         <v>4783.2825000000003</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="M23" s="8">
         <v>858661.89</v>
@@ -1877,7 +1885,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="6">
         <v>43573</v>
@@ -1903,14 +1911,14 @@
       <c r="I24" s="8">
         <v>6137.3806999999997</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="L24" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="M24" s="8">
         <v>1281522.79</v>
@@ -1938,269 +1946,275 @@
       </c>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="12"/>
-      <c r="S25" s="4" t="s">
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="15" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-    </row>
-    <row r="33" spans="1:19">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-    </row>
-    <row r="34" spans="1:19">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-    </row>
-    <row r="35" spans="1:19">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-    </row>
-    <row r="36" spans="1:19">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
-    </row>
-    <row r="37" spans="1:19">
-      <c r="A37" s="14" t="s">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A10:R10"/>
+    <mergeCell ref="A11:S11"/>
+    <mergeCell ref="A25:R25"/>
+    <mergeCell ref="A27:S36"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="K37:S37"/>
     <mergeCell ref="C1:S1"/>
     <mergeCell ref="C2:S3"/>
     <mergeCell ref="A7:S7"/>
@@ -2212,12 +2226,6 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A10:R10"/>
-    <mergeCell ref="A11:S11"/>
-    <mergeCell ref="A25:R25"/>
-    <mergeCell ref="A27:S36"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="K37:S37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>